<commit_message>
menambahkan fitur untuk verifikasi e-kin, dengan memasukkan username dan password verifikator, bot akan memverifikasi pengesahan aktivitas
</commit_message>
<xml_diff>
--- a/ekin.xlsx
+++ b/ekin.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24701"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="25629"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\laragon\www\python\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Develope\bot-ekin-sibon\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3DCDFAE7-3B7F-41D8-B847-D61D1DCE686A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{631B7F47-C022-489E-9FBC-64E5E2ED69C5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="21270" yWindow="780" windowWidth="21600" windowHeight="11835" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13176" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="6">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="8">
   <si>
     <t>taggal</t>
   </si>
@@ -43,6 +43,12 @@
   </si>
   <si>
     <t>11-10-2022</t>
+  </si>
+  <si>
+    <t>xxxx</t>
+  </si>
+  <si>
+    <t>yyyy</t>
   </si>
 </sst>
 </file>
@@ -367,54 +373,48 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:D4"/>
+  <dimension ref="A1:D5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A4" sqref="A4"/>
+      <selection activeCell="B1" sqref="B1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="20.5703125" customWidth="1"/>
-    <col min="2" max="2" width="19.42578125" customWidth="1"/>
-    <col min="3" max="3" width="15.7109375" customWidth="1"/>
-    <col min="4" max="4" width="11.85546875" customWidth="1"/>
+    <col min="1" max="1" width="20.5546875" customWidth="1"/>
+    <col min="2" max="2" width="19.44140625" customWidth="1"/>
+    <col min="3" max="3" width="15.6640625" customWidth="1"/>
+    <col min="4" max="4" width="11.88671875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
+        <v>6</v>
+      </c>
+      <c r="B1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A2" t="s">
         <v>0</v>
       </c>
-      <c r="B1" t="s">
+      <c r="B2" t="s">
         <v>1</v>
       </c>
-      <c r="C1" t="s">
+      <c r="C2" t="s">
         <v>2</v>
       </c>
-      <c r="D1" t="s">
+      <c r="D2" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A2" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="B2">
-        <v>1940</v>
-      </c>
-      <c r="C2">
-        <v>1</v>
-      </c>
-      <c r="D2" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A3" s="1" t="s">
         <v>5</v>
       </c>
       <c r="B3">
-        <v>122</v>
+        <v>1940</v>
       </c>
       <c r="C3">
         <v>1</v>
@@ -423,17 +423,31 @@
         <v>4</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A4" s="1" t="s">
         <v>5</v>
       </c>
       <c r="B4">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="C4">
         <v>1</v>
       </c>
       <c r="D4" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A5" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="B5">
+        <v>123</v>
+      </c>
+      <c r="C5">
+        <v>1</v>
+      </c>
+      <c r="D5" t="s">
         <v>4</v>
       </c>
     </row>

</xml_diff>